<commit_message>
rough draft of documentation added
</commit_message>
<xml_diff>
--- a/manufacturing/BOM.xlsx
+++ b/manufacturing/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/pyControl/pyControl_DSeries/manufacturing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/pyControl/DSeries_breakout/manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85256974-D856-6D44-BBCE-B1FDAA67879B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D41D70C-7944-994C-8364-4688971F4505}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24000" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pyboardbreakout" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>Qty</t>
   </si>
@@ -79,9 +79,6 @@
     <t>B3F-4000</t>
   </si>
   <si>
-    <t>Tactile Switch</t>
-  </si>
-  <si>
     <t>5V Linear Regulator</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>https://www.digikey.com/product-detail/en/toshiba-semiconductor-and-storage/TBD62083AFNGEL/TBD62083AFNGELCT-ND/5514123</t>
   </si>
   <si>
-    <t>PyControl D-Series Breakout 1.0</t>
-  </si>
-  <si>
     <t>PyControl D-Series Breakout PCB</t>
   </si>
   <si>
@@ -121,9 +115,6 @@
     <t>https://www.digikey.com/products/en?keywords=B3F-4000</t>
   </si>
   <si>
-    <t>tactile_switch.pdf</t>
-  </si>
-  <si>
     <t>DIN_clip.pdf</t>
   </si>
   <si>
@@ -170,6 +161,30 @@
   </si>
   <si>
     <t>DF40HC(4.0)-40DS-0.4V(70)</t>
+  </si>
+  <si>
+    <t>PyControl D-Series Breakout 1.1</t>
+  </si>
+  <si>
+    <t>Large Button</t>
+  </si>
+  <si>
+    <t>Small Button</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=sw1440ct</t>
+  </si>
+  <si>
+    <t>tactile_switch_large.pdf</t>
+  </si>
+  <si>
+    <t>tactile_switch_small.pdf</t>
+  </si>
+  <si>
+    <t>B3FS-1010P</t>
+  </si>
+  <si>
+    <t>https://oshpark.com/shared_projects/x12GQ4xq</t>
   </si>
 </sst>
 </file>
@@ -558,7 +573,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -598,11 +613,11 @@
       </c>
       <c r="C2" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!C2),"",IF(ISBLANK(pyboardbreakout_data!D2),pyboardbreakout_data!C2,CONCATENATE(" :download:`",pyboardbreakout_data!C2,"&lt;Datasheets/",pyboardbreakout_data!D2,"&gt;`")))</f>
-        <v>PyControl D-Series Breakout 1.0</v>
+        <v>PyControl D-Series Breakout 1.1</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F2),"",CONCATENATE("`",pyboardbreakout_data!E2," &lt;",pyboardbreakout_data!F2,"&gt;`__"))</f>
-        <v/>
+        <v>`OSH Park &lt;https://oshpark.com/shared_projects/x12GQ4xq&gt;`__</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -615,8 +630,8 @@
         <v>DIN Rail Adapter</v>
       </c>
       <c r="C3" t="str">
-        <f>IF(ISBLANK(pyboardbreakout_data!C3),"",IF(ISBLANK(pyboardbreakout_data!D3),pyboardbreakout_data!C3,CONCATENATE(" :download:`",pyboardbreakout_data!C3,"&lt;Datasheets/",pyboardbreakout_data!D3,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`1201578&lt;Datasheets/DIN_clip.pdf&gt;`</v>
+        <f>IF(ISBLANK(pyboardbreakout_data!C3),"",IF(ISBLANK(pyboardbreakout_data!D3),pyboardbreakout_data!C3,CONCATENATE(" :download:`",pyboardbreakout_data!C3,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D3,"&gt;`")))</f>
+        <v xml:space="preserve"> :download:`1201578&lt;../../manufacturing/datasheets/DIN_clip.pdf&gt;`</v>
       </c>
       <c r="D3" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F3),"",CONCATENATE("`",pyboardbreakout_data!E3," &lt;",pyboardbreakout_data!F3,"&gt;`__"))</f>
@@ -626,15 +641,15 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="str">
         <f>pyboardbreakout_data!A4</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="str">
         <f>pyboardbreakout_data!B4</f>
-        <v>Tactile Switch</v>
+        <v>Large Button</v>
       </c>
       <c r="C4" t="str">
-        <f>IF(ISBLANK(pyboardbreakout_data!C4),"",IF(ISBLANK(pyboardbreakout_data!D4),pyboardbreakout_data!C4,CONCATENATE(" :download:`",pyboardbreakout_data!C4,"&lt;Datasheets/",pyboardbreakout_data!D4,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`B3F-4000&lt;Datasheets/tactile_switch.pdf&gt;`</v>
+        <f>IF(ISBLANK(pyboardbreakout_data!C4),"",IF(ISBLANK(pyboardbreakout_data!D4),pyboardbreakout_data!C4,CONCATENATE(" :download:`",pyboardbreakout_data!C4,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D4,"&gt;`")))</f>
+        <v xml:space="preserve"> :download:`B3F-4000&lt;../../manufacturing/datasheets/tactile_switch_large.pdf&gt;`</v>
       </c>
       <c r="D4" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F4),"",CONCATENATE("`",pyboardbreakout_data!E4," &lt;",pyboardbreakout_data!F4,"&gt;`__"))</f>
@@ -642,111 +657,129 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <f>pyboardbreakout_data!A7</f>
+      <c r="A5" s="2" t="str">
+        <f>pyboardbreakout_data!A5</f>
         <v>1</v>
       </c>
       <c r="B5" t="str">
-        <f>pyboardbreakout_data!B7</f>
-        <v>5V Linear Regulator</v>
+        <f>pyboardbreakout_data!B5</f>
+        <v>Small Button</v>
       </c>
       <c r="C5" t="str">
-        <f>IF(ISBLANK(pyboardbreakout_data!C7),"",IF(ISBLANK(pyboardbreakout_data!D7),pyboardbreakout_data!C7,CONCATENATE(" :download:`",pyboardbreakout_data!C7,"&lt;Datasheets/",pyboardbreakout_data!D7,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`MC7805BDTRKG&lt;Datasheets/regulator.pdf&gt;`</v>
+        <f>IF(ISBLANK(pyboardbreakout_data!C5),"",IF(ISBLANK(pyboardbreakout_data!D5),pyboardbreakout_data!C5,CONCATENATE(" :download:`",pyboardbreakout_data!C5,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D5,"&gt;`")))</f>
+        <v xml:space="preserve"> :download:`B3FS-1010P&lt;../../manufacturing/datasheets/tactile_switch_small.pdf&gt;`</v>
       </c>
       <c r="D5" t="str">
-        <f>IF(ISBLANK(pyboardbreakout_data!F7),"",CONCATENATE("`",pyboardbreakout_data!E7," &lt;",pyboardbreakout_data!F7,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/on-semiconductor/MC7805BDTRKG/MC7805BDTRKGOSCT-ND/1139742&gt;`__</v>
+        <f>IF(ISBLANK(pyboardbreakout_data!F5),"",CONCATENATE("`",pyboardbreakout_data!E5," &lt;",pyboardbreakout_data!F5,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=sw1440ct&gt;`__</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="str">
-        <f>pyboardbreakout_data!A8</f>
-        <v>3</v>
-      </c>
-      <c r="B6" t="str">
-        <f>pyboardbreakout_data!B8</f>
-        <v>Transistor Array</v>
-      </c>
-      <c r="C6" t="str">
-        <f>IF(ISBLANK(pyboardbreakout_data!C8),"",IF(ISBLANK(pyboardbreakout_data!D8),pyboardbreakout_data!C8,CONCATENATE(" :download:`",pyboardbreakout_data!C8,"&lt;datasheets/",pyboardbreakout_data!D8,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`TBD62083AFNG&lt;datasheets/transistor_array.pdf&gt;`</v>
-      </c>
-      <c r="D6" t="str">
-        <f>IF(ISBLANK(pyboardbreakout_data!F8),"",CONCATENATE("`",pyboardbreakout_data!E8," &lt;",pyboardbreakout_data!F8,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/toshiba-semiconductor-and-storage/TBD62083AFNGEL/TBD62083AFNGELCT-ND/5514123&gt;`__</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="str">
-        <f>pyboardbreakout_data!A9</f>
-        <v>1</v>
-      </c>
-      <c r="B7" t="str">
-        <f>pyboardbreakout_data!B9</f>
-        <v>Diode</v>
-      </c>
-      <c r="C7" t="str">
-        <f>IF(ISBLANK(pyboardbreakout_data!C9),"",IF(ISBLANK(pyboardbreakout_data!D9),pyboardbreakout_data!C9,CONCATENATE(" :download:`",pyboardbreakout_data!C9,"&lt;datasheets/",pyboardbreakout_data!D9,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`MBR120VLSFT3G&lt;datasheets/diode.pdf&gt;`</v>
-      </c>
-      <c r="D7" t="str">
-        <f>IF(ISBLANK(pyboardbreakout_data!F9),"",CONCATENATE("`",pyboardbreakout_data!E9," &lt;",pyboardbreakout_data!F9,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/on-semiconductor/MBR120VLSFT3G/MBR120VLSFT3GOSCT-ND/3487322&gt;`__</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="str">
-        <f>pyboardbreakout_data!A10</f>
-        <v>2</v>
-      </c>
-      <c r="B8" t="str">
-        <f>pyboardbreakout_data!B10</f>
-        <v>1µF 25V Capacitor (1206)</v>
-      </c>
-      <c r="C8" t="str">
-        <f>IF(ISBLANK(pyboardbreakout_data!C10),"",IF(ISBLANK(pyboardbreakout_data!D10),pyboardbreakout_data!C10,CONCATENATE(" :download:`",pyboardbreakout_data!C10,"&lt;datasheets/",pyboardbreakout_data!D10,"&gt;`")))</f>
-        <v/>
-      </c>
-      <c r="D8" t="str">
-        <f>IF(ISBLANK(pyboardbreakout_data!F10),"",CONCATENATE("`",pyboardbreakout_data!E10," &lt;",pyboardbreakout_data!F10,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/C1206C105K3RACTU/399-1255-1-ND/411530/?itemSeq=290616497&gt;`__</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <f>pyboardbreakout_data!A5</f>
-        <v>2</v>
-      </c>
-      <c r="B9" t="str">
-        <f>pyboardbreakout_data!B5</f>
-        <v>12-Port RJ45 Connector</v>
-      </c>
-      <c r="C9" t="str">
-        <f>IF(ISBLANK(pyboardbreakout_data!C5),"",IF(ISBLANK(pyboardbreakout_data!D5),pyboardbreakout_data!C5,CONCATENATE(" :download:`",pyboardbreakout_data!C5,"&lt;datasheets/",pyboardbreakout_data!D5,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`5569263-1&lt;datasheets/rj45_12port.pdf&gt;`</v>
-      </c>
-      <c r="D9" t="str">
-        <f>IF(ISBLANK(pyboardbreakout_data!F5),"",CONCATENATE("`",pyboardbreakout_data!E5," &lt;",pyboardbreakout_data!F5,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=5569263&gt;`__</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A6" s="2">
         <f>pyboardbreakout_data!A6</f>
         <v>2</v>
       </c>
+      <c r="B6" t="str">
+        <f>pyboardbreakout_data!B6</f>
+        <v>12-Port RJ45 Connector</v>
+      </c>
+      <c r="C6" t="str">
+        <f>IF(ISBLANK(pyboardbreakout_data!C6),"",IF(ISBLANK(pyboardbreakout_data!D6),pyboardbreakout_data!C6,CONCATENATE(" :download:`",pyboardbreakout_data!C6,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D6,"&gt;`")))</f>
+        <v xml:space="preserve"> :download:`5569263-1&lt;../../manufacturing/datasheets/rj45_12port.pdf&gt;`</v>
+      </c>
+      <c r="D6" t="str">
+        <f>IF(ISBLANK(pyboardbreakout_data!F6),"",CONCATENATE("`",pyboardbreakout_data!E6," &lt;",pyboardbreakout_data!F6,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=5569263&gt;`__</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <f>pyboardbreakout_data!A7</f>
+        <v>2</v>
+      </c>
+      <c r="B7" t="str">
+        <f>pyboardbreakout_data!B7</f>
+        <v>40-pin WBUS connector</v>
+      </c>
+      <c r="C7" t="str">
+        <f>IF(ISBLANK(pyboardbreakout_data!C7),"",IF(ISBLANK(pyboardbreakout_data!D7),pyboardbreakout_data!C7,CONCATENATE(" :download:`",pyboardbreakout_data!C7,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D7,"&gt;`")))</f>
+        <v xml:space="preserve"> :download:`DF40HC(4.0)-40DS-0.4V(70)&lt;../../manufacturing/datasheets/40_pin_connector.pdf&gt;`</v>
+      </c>
+      <c r="D7" t="str">
+        <f>IF(ISBLANK(pyboardbreakout_data!F7),"",CONCATENATE("`",pyboardbreakout_data!E7," &lt;",pyboardbreakout_data!F7,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/DF40HC(4.0)-40DS-0.4V(70)/H124604CT-ND/5155907/?itemSeq=290724516&gt;`__</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <f>pyboardbreakout_data!A8</f>
+        <v>1</v>
+      </c>
+      <c r="B8" t="str">
+        <f>pyboardbreakout_data!B8</f>
+        <v>5V Linear Regulator</v>
+      </c>
+      <c r="C8" t="str">
+        <f>IF(ISBLANK(pyboardbreakout_data!C8),"",IF(ISBLANK(pyboardbreakout_data!D8),pyboardbreakout_data!C8,CONCATENATE(" :download:`",pyboardbreakout_data!C8,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D8,"&gt;`")))</f>
+        <v xml:space="preserve"> :download:`MC7805BDTRKG&lt;../../manufacturing/datasheets/regulator.pdf&gt;`</v>
+      </c>
+      <c r="D8" t="str">
+        <f>IF(ISBLANK(pyboardbreakout_data!F8),"",CONCATENATE("`",pyboardbreakout_data!E8," &lt;",pyboardbreakout_data!F8,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/on-semiconductor/MC7805BDTRKG/MC7805BDTRKGOSCT-ND/1139742&gt;`__</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="str">
+        <f>pyboardbreakout_data!A9</f>
+        <v>3</v>
+      </c>
+      <c r="B9" t="str">
+        <f>pyboardbreakout_data!B9</f>
+        <v>Transistor Array</v>
+      </c>
+      <c r="C9" t="str">
+        <f>IF(ISBLANK(pyboardbreakout_data!C9),"",IF(ISBLANK(pyboardbreakout_data!D9),pyboardbreakout_data!C9,CONCATENATE(" :download:`",pyboardbreakout_data!C9,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D9,"&gt;`")))</f>
+        <v xml:space="preserve"> :download:`TBD62083AFNG&lt;../../manufacturing/datasheets/transistor_array.pdf&gt;`</v>
+      </c>
+      <c r="D9" t="str">
+        <f>IF(ISBLANK(pyboardbreakout_data!F9),"",CONCATENATE("`",pyboardbreakout_data!E9," &lt;",pyboardbreakout_data!F9,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/toshiba-semiconductor-and-storage/TBD62083AFNGEL/TBD62083AFNGELCT-ND/5514123&gt;`__</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="str">
+        <f>pyboardbreakout_data!A10</f>
+        <v>1</v>
+      </c>
       <c r="B10" t="str">
-        <f>pyboardbreakout_data!B6</f>
-        <v>40-pin WBUS connector</v>
+        <f>pyboardbreakout_data!B10</f>
+        <v>Diode</v>
       </c>
       <c r="C10" t="str">
-        <f>IF(ISBLANK(pyboardbreakout_data!C6),"",IF(ISBLANK(pyboardbreakout_data!D6),pyboardbreakout_data!C6,CONCATENATE(" :download:`",pyboardbreakout_data!C6,"&lt;datasheets/",pyboardbreakout_data!D6,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`DF40HC(4.0)-40DS-0.4V(70)&lt;datasheets/40_pin_connector.pdf&gt;`</v>
+        <f>IF(ISBLANK(pyboardbreakout_data!C10),"",IF(ISBLANK(pyboardbreakout_data!D10),pyboardbreakout_data!C10,CONCATENATE(" :download:`",pyboardbreakout_data!C10,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D10,"&gt;`")))</f>
+        <v xml:space="preserve"> :download:`MBR120VLSFT3G&lt;../../manufacturing/datasheets/diode.pdf&gt;`</v>
       </c>
       <c r="D10" t="str">
-        <f>IF(ISBLANK(pyboardbreakout_data!F6),"",CONCATENATE("`",pyboardbreakout_data!E6," &lt;",pyboardbreakout_data!F6,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/DF40HC(4.0)-40DS-0.4V(70)/H124604CT-ND/5155907/?itemSeq=290724516&gt;`__</v>
+        <f>IF(ISBLANK(pyboardbreakout_data!F10),"",CONCATENATE("`",pyboardbreakout_data!E10," &lt;",pyboardbreakout_data!F10,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/on-semiconductor/MBR120VLSFT3G/MBR120VLSFT3GOSCT-ND/3487322&gt;`__</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="str">
+        <f>pyboardbreakout_data!A11</f>
+        <v>2</v>
+      </c>
+      <c r="B11" t="str">
+        <f>pyboardbreakout_data!B11</f>
+        <v>1µF 25V Capacitor (1206)</v>
+      </c>
+      <c r="C11" t="str">
+        <f>IF(ISBLANK(pyboardbreakout_data!C11),"",IF(ISBLANK(pyboardbreakout_data!D11),pyboardbreakout_data!C11,CONCATENATE(" :download:`",pyboardbreakout_data!C11,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D11,"&gt;`")))</f>
+        <v/>
+      </c>
+      <c r="D11" t="str">
+        <f>IF(ISBLANK(pyboardbreakout_data!F11),"",CONCATENATE("`",pyboardbreakout_data!E11," &lt;",pyboardbreakout_data!F11,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/C1206C105K3RACTU/399-1255-1-ND/411530/?itemSeq=290616497&gt;`__</v>
       </c>
     </row>
     <row r="40" hidden="1" x14ac:dyDescent="0.2"/>
@@ -760,10 +793,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F118"/>
+  <dimension ref="A1:F119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -806,13 +839,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -820,59 +856,59 @@
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>2</v>
+      <c r="A5" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -880,10 +916,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>30</v>
@@ -892,91 +928,106 @@
         <v>9</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C11" s="3"/>
-      <c r="F11"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="E16" s="4"/>
+      <c r="F11" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C12" s="3"/>
+      <c r="F12"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="5"/>
@@ -984,6 +1035,8 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
@@ -998,8 +1051,8 @@
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E22" s="4"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C26" s="6"/>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E23" s="4"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C27" s="6"/>
@@ -1034,19 +1087,24 @@
     <row r="37" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C37" s="6"/>
     </row>
-    <row r="118" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F118" s="3"/>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C38" s="6"/>
+    </row>
+    <row r="119" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F119" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" xr:uid="{4D814F7E-E809-044B-A9CF-7ABAEE328861}"/>
+    <hyperlink ref="F9" r:id="rId1" xr:uid="{4D814F7E-E809-044B-A9CF-7ABAEE328861}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{05B760F1-2263-9849-9E96-16FABD4435DD}"/>
     <hyperlink ref="F4" r:id="rId3" xr:uid="{297095E6-C369-9C43-87E4-9EE7FC3E90F5}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{A882F800-A73F-C940-828A-850803EE1E9B}"/>
-    <hyperlink ref="F9" r:id="rId5" xr:uid="{A4565103-D08B-9C42-B67C-AD72348CE1F4}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{84379817-83EA-074E-96CF-155977A8D9F8}"/>
-    <hyperlink ref="F10" r:id="rId7" xr:uid="{AEF59290-E6FC-064F-A693-61CD54A5FD6A}"/>
-    <hyperlink ref="F6" r:id="rId8" xr:uid="{38251BF6-DAAA-094A-96E3-B456AE1F7870}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{A882F800-A73F-C940-828A-850803EE1E9B}"/>
+    <hyperlink ref="F10" r:id="rId5" xr:uid="{A4565103-D08B-9C42-B67C-AD72348CE1F4}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{84379817-83EA-074E-96CF-155977A8D9F8}"/>
+    <hyperlink ref="F11" r:id="rId7" xr:uid="{AEF59290-E6FC-064F-A693-61CD54A5FD6A}"/>
+    <hyperlink ref="F7" r:id="rId8" xr:uid="{38251BF6-DAAA-094A-96E3-B456AE1F7870}"/>
+    <hyperlink ref="F5" r:id="rId9" xr:uid="{545989D7-5B32-5E4D-B4BD-757D46D9341E}"/>
+    <hyperlink ref="F2" r:id="rId10" xr:uid="{F603E055-EBEC-EB49-8C97-D0FCC8E14D99}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Revised PCB to v1.2 Switched from linear regulator to DC-DC converter. 1µF capacitors are now 10µF. Added TAPR link to silkscreen and schematic.
</commit_message>
<xml_diff>
--- a/manufacturing/BOM.xlsx
+++ b/manufacturing/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/pyControl/DSeries_breakout/manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D41D70C-7944-994C-8364-4688971F4505}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9255FBF7-08A3-A246-ADBD-E6528D537118}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pyboardbreakout" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,6 @@
     <t>B3F-4000</t>
   </si>
   <si>
-    <t>5V Linear Regulator</t>
-  </si>
-  <si>
     <t>Transistor Array</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>12-Port RJ45 Connector</t>
   </si>
   <si>
-    <t>40-pin WBUS connector</t>
-  </si>
-  <si>
     <t>transistor_array.pdf</t>
   </si>
   <si>
@@ -142,21 +136,9 @@
     <t>diode.pdf</t>
   </si>
   <si>
-    <t>MC7805BDTRKG</t>
-  </si>
-  <si>
-    <t>regulator.pdf</t>
-  </si>
-  <si>
     <t>MBR120VLSFT3G</t>
   </si>
   <si>
-    <t>1µF 25V Capacitor (1206)</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/C1206C105K3RACTU/399-1255-1-ND/411530/?itemSeq=290616497</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/product-detail/en/DF40HC(4.0)-40DS-0.4V(70)/H124604CT-ND/5155907/?itemSeq=290724516</t>
   </si>
   <si>
@@ -185,6 +167,24 @@
   </si>
   <si>
     <t>https://oshpark.com/shared_projects/x12GQ4xq</t>
+  </si>
+  <si>
+    <t>10µF 25V Capacitor (1206)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=1276-1804-1-ND</t>
+  </si>
+  <si>
+    <t>40-pin WBUS Connector</t>
+  </si>
+  <si>
+    <t>5V DC to DC Converter</t>
+  </si>
+  <si>
+    <t>R-78E5.0-1.0</t>
+  </si>
+  <si>
+    <t>dc_converter.pdf</t>
   </si>
 </sst>
 </file>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -699,7 +699,7 @@
       </c>
       <c r="B7" t="str">
         <f>pyboardbreakout_data!B7</f>
-        <v>40-pin WBUS connector</v>
+        <v>40-pin WBUS Connector</v>
       </c>
       <c r="C7" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!C7),"",IF(ISBLANK(pyboardbreakout_data!D7),pyboardbreakout_data!C7,CONCATENATE(" :download:`",pyboardbreakout_data!C7,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D7,"&gt;`")))</f>
@@ -717,11 +717,11 @@
       </c>
       <c r="B8" t="str">
         <f>pyboardbreakout_data!B8</f>
-        <v>5V Linear Regulator</v>
+        <v>5V DC to DC Converter</v>
       </c>
       <c r="C8" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!C8),"",IF(ISBLANK(pyboardbreakout_data!D8),pyboardbreakout_data!C8,CONCATENATE(" :download:`",pyboardbreakout_data!C8,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D8,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`MC7805BDTRKG&lt;../../manufacturing/datasheets/regulator.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`R-78E5.0-1.0&lt;../../manufacturing/datasheets/dc_converter.pdf&gt;`</v>
       </c>
       <c r="D8" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F8),"",CONCATENATE("`",pyboardbreakout_data!E8," &lt;",pyboardbreakout_data!F8,"&gt;`__"))</f>
@@ -771,7 +771,7 @@
       </c>
       <c r="B11" t="str">
         <f>pyboardbreakout_data!B11</f>
-        <v>1µF 25V Capacitor (1206)</v>
+        <v>10µF 25V Capacitor (1206)</v>
       </c>
       <c r="C11" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!C11),"",IF(ISBLANK(pyboardbreakout_data!D11),pyboardbreakout_data!C11,CONCATENATE(" :download:`",pyboardbreakout_data!C11,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D11,"&gt;`")))</f>
@@ -779,7 +779,7 @@
       </c>
       <c r="D11" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F11),"",CONCATENATE("`",pyboardbreakout_data!E11," &lt;",pyboardbreakout_data!F11,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/C1206C105K3RACTU/399-1255-1-ND/411530/?itemSeq=290616497&gt;`__</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=1276-1804-1-ND&gt;`__</v>
       </c>
     </row>
     <row r="40" hidden="1" x14ac:dyDescent="0.2"/>
@@ -795,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -839,16 +839,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -856,19 +856,19 @@
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -876,19 +876,19 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -896,19 +896,19 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -916,19 +916,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -936,19 +936,19 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -956,19 +956,19 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -976,19 +976,19 @@
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -996,19 +996,19 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1016,13 +1016,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1101,10 +1101,10 @@
     <hyperlink ref="F6" r:id="rId4" xr:uid="{A882F800-A73F-C940-828A-850803EE1E9B}"/>
     <hyperlink ref="F10" r:id="rId5" xr:uid="{A4565103-D08B-9C42-B67C-AD72348CE1F4}"/>
     <hyperlink ref="F8" r:id="rId6" xr:uid="{84379817-83EA-074E-96CF-155977A8D9F8}"/>
-    <hyperlink ref="F11" r:id="rId7" xr:uid="{AEF59290-E6FC-064F-A693-61CD54A5FD6A}"/>
-    <hyperlink ref="F7" r:id="rId8" xr:uid="{38251BF6-DAAA-094A-96E3-B456AE1F7870}"/>
-    <hyperlink ref="F5" r:id="rId9" xr:uid="{545989D7-5B32-5E4D-B4BD-757D46D9341E}"/>
-    <hyperlink ref="F2" r:id="rId10" xr:uid="{F603E055-EBEC-EB49-8C97-D0FCC8E14D99}"/>
+    <hyperlink ref="F7" r:id="rId7" xr:uid="{38251BF6-DAAA-094A-96E3-B456AE1F7870}"/>
+    <hyperlink ref="F5" r:id="rId8" xr:uid="{545989D7-5B32-5E4D-B4BD-757D46D9341E}"/>
+    <hyperlink ref="F2" r:id="rId9" xr:uid="{F603E055-EBEC-EB49-8C97-D0FCC8E14D99}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{079AE725-A048-B84F-ACEE-69047962AE7F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
pcb version 1.3. W1 cannot be used as DIO, so now B4_COMA is connected to pin9 (W9). W69 cannot be used as DIO, so now B5_COMB is connected to pin5 (W5). Added microusb connector so that you can permanently plug into breakout board and talk to the pyboard via the Hirose connector. This enables usb communication with the pyboard while still allowing one to easily swap out pyboards if necessary. changed user switch to SMD part Shifted components around.
</commit_message>
<xml_diff>
--- a/manufacturing/BOM.xlsx
+++ b/manufacturing/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/pyControl/DSeries_breakout/manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F268EEA-3F44-514B-9F55-B4C82111EE23}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DF6E68-8106-704D-8517-C826675B323C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3460" windowWidth="24000" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="460" windowWidth="24000" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pyboardbreakout" sheetId="1" r:id="rId1"/>
@@ -127,9 +127,6 @@
     <t>https://www.digikey.com/product-detail/en/on-semiconductor/MBR120VLSFT3G/MBR120VLSFT3GOSCT-ND/3487322</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/on-semiconductor/MC7805BDTRKG/MC7805BDTRKGOSCT-ND/1139742</t>
-  </si>
-  <si>
     <t>diode.pdf</t>
   </si>
   <si>
@@ -188,6 +185,9 @@
   </si>
   <si>
     <t>Printed Circuit Board</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=945-2201-ND</t>
   </si>
 </sst>
 </file>
@@ -728,7 +728,7 @@
       </c>
       <c r="D8" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F8),"",CONCATENATE("`",pyboardbreakout_data!E8," &lt;",pyboardbreakout_data!F8,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/on-semiconductor/MC7805BDTRKG/MC7805BDTRKGOSCT-ND/1139742&gt;`__</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=945-2201-ND&gt;`__</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -842,19 +842,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -882,13 +882,13 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
@@ -902,19 +902,19 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -942,10 +942,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>24</v>
@@ -954,7 +954,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -962,19 +962,19 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1005,10 +1005,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>9</v>
@@ -1022,13 +1022,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1106,7 +1106,7 @@
     <hyperlink ref="F4" r:id="rId3" xr:uid="{297095E6-C369-9C43-87E4-9EE7FC3E90F5}"/>
     <hyperlink ref="F6" r:id="rId4" xr:uid="{A882F800-A73F-C940-828A-850803EE1E9B}"/>
     <hyperlink ref="F10" r:id="rId5" xr:uid="{A4565103-D08B-9C42-B67C-AD72348CE1F4}"/>
-    <hyperlink ref="F8" r:id="rId6" xr:uid="{84379817-83EA-074E-96CF-155977A8D9F8}"/>
+    <hyperlink ref="F8" r:id="rId6" display="https://www.digikey.com/product-detail/en/on-semiconductor/MC7805BDTRKG/MC7805BDTRKGOSCT-ND/1139742" xr:uid="{84379817-83EA-074E-96CF-155977A8D9F8}"/>
     <hyperlink ref="F7" r:id="rId7" xr:uid="{38251BF6-DAAA-094A-96E3-B456AE1F7870}"/>
     <hyperlink ref="F5" r:id="rId8" xr:uid="{545989D7-5B32-5E4D-B4BD-757D46D9341E}"/>
     <hyperlink ref="F2" r:id="rId9" display="https://oshpark.com/shared_projects/x12GQ4xq" xr:uid="{F603E055-EBEC-EB49-8C97-D0FCC8E14D99}"/>

</xml_diff>

<commit_message>
updated docs for v1.3
</commit_message>
<xml_diff>
--- a/manufacturing/BOM.xlsx
+++ b/manufacturing/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/pyControl/DSeries_breakout/manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DF6E68-8106-704D-8517-C826675B323C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A292DF0F-A0D5-0349-A297-F91DC131A439}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="460" windowWidth="24000" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="pyboardbreakout" sheetId="1" r:id="rId1"/>
     <sheet name="pyboardbreakout_data" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
   <si>
     <t>Qty</t>
   </si>
@@ -76,9 +76,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>B3F-4000</t>
-  </si>
-  <si>
     <t>Transistor Array</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>1201578</t>
   </si>
   <si>
-    <t>https://www.digikey.com/products/en?keywords=B3F-4000</t>
-  </si>
-  <si>
     <t>DIN_clip.pdf</t>
   </si>
   <si>
@@ -188,6 +182,24 @@
   </si>
   <si>
     <t>https://www.digikey.com/products/en?keywords=945-2201-ND</t>
+  </si>
+  <si>
+    <t>PJ-037A</t>
+  </si>
+  <si>
+    <t>Barrel Jack Connector</t>
+  </si>
+  <si>
+    <t>barrel_jack.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=CP-037A-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=EG4906CT-ND</t>
+  </si>
+  <si>
+    <t>TL3300DF160Q</t>
   </si>
 </sst>
 </file>
@@ -576,7 +588,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C2:C3"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -652,11 +664,11 @@
       </c>
       <c r="C4" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!C4),"",IF(ISBLANK(pyboardbreakout_data!D4),pyboardbreakout_data!C4,CONCATENATE(" :download:`",pyboardbreakout_data!C4,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D4,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`B3F-4000&lt;../../manufacturing/datasheets/tactile_switch_large.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`TL3300DF160Q&lt;../../manufacturing/datasheets/tactile_switch_large.pdf&gt;`</v>
       </c>
       <c r="D4" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F4),"",CONCATENATE("`",pyboardbreakout_data!E4," &lt;",pyboardbreakout_data!F4,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=B3F-4000&gt;`__</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=EG4906CT-ND&gt;`__</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -678,21 +690,21 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="2" t="str">
         <f>pyboardbreakout_data!A6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="str">
         <f>pyboardbreakout_data!B6</f>
-        <v>12-Port RJ45 Connector</v>
+        <v>Barrel Jack Connector</v>
       </c>
       <c r="C6" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!C6),"",IF(ISBLANK(pyboardbreakout_data!D6),pyboardbreakout_data!C6,CONCATENATE(" :download:`",pyboardbreakout_data!C6,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D6,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`5569263-1&lt;../../manufacturing/datasheets/rj45_12port.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`PJ-037A&lt;../../manufacturing/datasheets/barrel_jack.pdf&gt;`</v>
       </c>
       <c r="D6" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F6),"",CONCATENATE("`",pyboardbreakout_data!E6," &lt;",pyboardbreakout_data!F6,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=5569263&gt;`__</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=CP-037A-ND&gt;`__</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -702,86 +714,104 @@
       </c>
       <c r="B7" t="str">
         <f>pyboardbreakout_data!B7</f>
-        <v>40-pin WBUS Connector</v>
+        <v>12-Port RJ45 Connector</v>
       </c>
       <c r="C7" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!C7),"",IF(ISBLANK(pyboardbreakout_data!D7),pyboardbreakout_data!C7,CONCATENATE(" :download:`",pyboardbreakout_data!C7,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D7,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`DF40HC(4.0)-40DS-0.4V(70)&lt;../../manufacturing/datasheets/40_pin_connector.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`5569263-1&lt;../../manufacturing/datasheets/rj45_12port.pdf&gt;`</v>
       </c>
       <c r="D7" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F7),"",CONCATENATE("`",pyboardbreakout_data!E7," &lt;",pyboardbreakout_data!F7,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/DF40HC(4.0)-40DS-0.4V(70)/H124604CT-ND/5155907/?itemSeq=290724516&gt;`__</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=5569263&gt;`__</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <f>pyboardbreakout_data!A8</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" t="str">
         <f>pyboardbreakout_data!B8</f>
-        <v>5V DC to DC Converter</v>
+        <v>40-pin WBUS Connector</v>
       </c>
       <c r="C8" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!C8),"",IF(ISBLANK(pyboardbreakout_data!D8),pyboardbreakout_data!C8,CONCATENATE(" :download:`",pyboardbreakout_data!C8,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D8,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`R-78E5.0-1.0&lt;../../manufacturing/datasheets/dc_converter.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`DF40HC(4.0)-40DS-0.4V(70)&lt;../../manufacturing/datasheets/40_pin_connector.pdf&gt;`</v>
       </c>
       <c r="D8" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F8),"",CONCATENATE("`",pyboardbreakout_data!E8," &lt;",pyboardbreakout_data!F8,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=945-2201-ND&gt;`__</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/DF40HC(4.0)-40DS-0.4V(70)/H124604CT-ND/5155907/?itemSeq=290724516&gt;`__</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="str">
+      <c r="A9" s="2">
         <f>pyboardbreakout_data!A9</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B9" t="str">
         <f>pyboardbreakout_data!B9</f>
-        <v>Transistor Array</v>
+        <v>5V DC to DC Converter</v>
       </c>
       <c r="C9" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!C9),"",IF(ISBLANK(pyboardbreakout_data!D9),pyboardbreakout_data!C9,CONCATENATE(" :download:`",pyboardbreakout_data!C9,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D9,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`TBD62083AFNG&lt;../../manufacturing/datasheets/transistor_array.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`R-78E5.0-1.0&lt;../../manufacturing/datasheets/dc_converter.pdf&gt;`</v>
       </c>
       <c r="D9" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F9),"",CONCATENATE("`",pyboardbreakout_data!E9," &lt;",pyboardbreakout_data!F9,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/toshiba-semiconductor-and-storage/TBD62083AFNGEL/TBD62083AFNGELCT-ND/5514123&gt;`__</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=945-2201-ND&gt;`__</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="str">
         <f>pyboardbreakout_data!A10</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B10" t="str">
         <f>pyboardbreakout_data!B10</f>
-        <v>Diode</v>
+        <v>Transistor Array</v>
       </c>
       <c r="C10" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!C10),"",IF(ISBLANK(pyboardbreakout_data!D10),pyboardbreakout_data!C10,CONCATENATE(" :download:`",pyboardbreakout_data!C10,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D10,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`MBR120VLSFT3G&lt;../../manufacturing/datasheets/diode.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`TBD62083AFNG&lt;../../manufacturing/datasheets/transistor_array.pdf&gt;`</v>
       </c>
       <c r="D10" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F10),"",CONCATENATE("`",pyboardbreakout_data!E10," &lt;",pyboardbreakout_data!F10,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/on-semiconductor/MBR120VLSFT3G/MBR120VLSFT3GOSCT-ND/3487322&gt;`__</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/toshiba-semiconductor-and-storage/TBD62083AFNGEL/TBD62083AFNGELCT-ND/5514123&gt;`__</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="str">
         <f>pyboardbreakout_data!A11</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" t="str">
         <f>pyboardbreakout_data!B11</f>
-        <v>10µF 25V Capacitor (1206)</v>
+        <v>Diode</v>
       </c>
       <c r="C11" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!C11),"",IF(ISBLANK(pyboardbreakout_data!D11),pyboardbreakout_data!C11,CONCATENATE(" :download:`",pyboardbreakout_data!C11,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D11,"&gt;`")))</f>
-        <v/>
+        <v xml:space="preserve"> :download:`MBR120VLSFT3G&lt;../../manufacturing/datasheets/diode.pdf&gt;`</v>
       </c>
       <c r="D11" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F11),"",CONCATENATE("`",pyboardbreakout_data!E11," &lt;",pyboardbreakout_data!F11,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/on-semiconductor/MBR120VLSFT3G/MBR120VLSFT3GOSCT-ND/3487322&gt;`__</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="str">
+        <f>pyboardbreakout_data!A12</f>
+        <v>2</v>
+      </c>
+      <c r="B12" t="str">
+        <f>pyboardbreakout_data!B12</f>
+        <v>10µF 25V Capacitor (1206)</v>
+      </c>
+      <c r="C12" t="str">
+        <f>IF(ISBLANK(pyboardbreakout_data!C12),"",IF(ISBLANK(pyboardbreakout_data!D12),pyboardbreakout_data!C12,CONCATENATE(" :download:`",pyboardbreakout_data!C12,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D12,"&gt;`")))</f>
+        <v/>
+      </c>
+      <c r="D12" t="str">
+        <f>IF(ISBLANK(pyboardbreakout_data!F12),"",CONCATENATE("`",pyboardbreakout_data!E12," &lt;",pyboardbreakout_data!F12,"&gt;`__"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=1276-1804-1-ND&gt;`__</v>
       </c>
     </row>
@@ -796,10 +826,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F119"/>
+  <dimension ref="A1:F120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -842,19 +872,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -862,19 +892,19 @@
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -882,19 +912,19 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -902,39 +932,39 @@
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>2</v>
+      <c r="A6" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -942,103 +972,118 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>12</v>
+      <c r="A9" s="2">
+        <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="B12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C12" s="3"/>
-      <c r="F12"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="E17" s="4"/>
+      <c r="F12" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C13" s="3"/>
+      <c r="F13"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="5"/>
@@ -1046,6 +1091,8 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
@@ -1060,8 +1107,8 @@
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E23" s="4"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C27" s="6"/>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E24" s="4"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C28" s="6"/>
@@ -1096,21 +1143,24 @@
     <row r="38" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C38" s="6"/>
     </row>
-    <row r="119" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F119" s="3"/>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="6"/>
+    </row>
+    <row r="120" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F120" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F9" r:id="rId1" xr:uid="{4D814F7E-E809-044B-A9CF-7ABAEE328861}"/>
+    <hyperlink ref="F10" r:id="rId1" xr:uid="{4D814F7E-E809-044B-A9CF-7ABAEE328861}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{05B760F1-2263-9849-9E96-16FABD4435DD}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{297095E6-C369-9C43-87E4-9EE7FC3E90F5}"/>
-    <hyperlink ref="F6" r:id="rId4" xr:uid="{A882F800-A73F-C940-828A-850803EE1E9B}"/>
-    <hyperlink ref="F10" r:id="rId5" xr:uid="{A4565103-D08B-9C42-B67C-AD72348CE1F4}"/>
-    <hyperlink ref="F8" r:id="rId6" display="https://www.digikey.com/product-detail/en/on-semiconductor/MC7805BDTRKG/MC7805BDTRKGOSCT-ND/1139742" xr:uid="{84379817-83EA-074E-96CF-155977A8D9F8}"/>
-    <hyperlink ref="F7" r:id="rId7" xr:uid="{38251BF6-DAAA-094A-96E3-B456AE1F7870}"/>
+    <hyperlink ref="F4" r:id="rId3" display="https://www.digikey.com/products/en?keywords=B3F-4000" xr:uid="{297095E6-C369-9C43-87E4-9EE7FC3E90F5}"/>
+    <hyperlink ref="F7" r:id="rId4" xr:uid="{A882F800-A73F-C940-828A-850803EE1E9B}"/>
+    <hyperlink ref="F11" r:id="rId5" xr:uid="{A4565103-D08B-9C42-B67C-AD72348CE1F4}"/>
+    <hyperlink ref="F9" r:id="rId6" display="https://www.digikey.com/product-detail/en/on-semiconductor/MC7805BDTRKG/MC7805BDTRKGOSCT-ND/1139742" xr:uid="{84379817-83EA-074E-96CF-155977A8D9F8}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{38251BF6-DAAA-094A-96E3-B456AE1F7870}"/>
     <hyperlink ref="F5" r:id="rId8" xr:uid="{545989D7-5B32-5E4D-B4BD-757D46D9341E}"/>
     <hyperlink ref="F2" r:id="rId9" display="https://oshpark.com/shared_projects/x12GQ4xq" xr:uid="{F603E055-EBEC-EB49-8C97-D0FCC8E14D99}"/>
-    <hyperlink ref="F11" r:id="rId10" xr:uid="{079AE725-A048-B84F-ACEE-69047962AE7F}"/>
+    <hyperlink ref="F12" r:id="rId10" xr:uid="{079AE725-A048-B84F-ACEE-69047962AE7F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
micro usb socket was missing from docs
</commit_message>
<xml_diff>
--- a/manufacturing/BOM.xlsx
+++ b/manufacturing/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/pyControl/DSeries_breakout/manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A292DF0F-A0D5-0349-A297-F91DC131A439}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CF704A-ED42-1941-8216-20B734A6E0F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="460" windowWidth="24000" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="460" windowWidth="24000" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pyboardbreakout" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>Qty</t>
   </si>
@@ -200,6 +200,18 @@
   </si>
   <si>
     <t>TL3300DF160Q</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=609-4618-1-ND</t>
+  </si>
+  <si>
+    <t>horz_µUSB.pdf</t>
+  </si>
+  <si>
+    <t>10118194-0001LF</t>
+  </si>
+  <si>
+    <t>Micro USB horizontal socket</t>
   </si>
 </sst>
 </file>
@@ -587,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -744,74 +756,92 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="2" t="str">
         <f>pyboardbreakout_data!A9</f>
         <v>1</v>
       </c>
       <c r="B9" t="str">
         <f>pyboardbreakout_data!B9</f>
-        <v>5V DC to DC Converter</v>
+        <v>Micro USB horizontal socket</v>
       </c>
       <c r="C9" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!C9),"",IF(ISBLANK(pyboardbreakout_data!D9),pyboardbreakout_data!C9,CONCATENATE(" :download:`",pyboardbreakout_data!C9,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D9,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`R-78E5.0-1.0&lt;../../manufacturing/datasheets/dc_converter.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`10118194-0001LF&lt;../../manufacturing/datasheets/horz_µUSB.pdf&gt;`</v>
       </c>
       <c r="D9" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F9),"",CONCATENATE("`",pyboardbreakout_data!E9," &lt;",pyboardbreakout_data!F9,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=945-2201-ND&gt;`__</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=609-4618-1-ND&gt;`__</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="str">
+      <c r="A10" s="2">
         <f>pyboardbreakout_data!A10</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B10" t="str">
         <f>pyboardbreakout_data!B10</f>
-        <v>Transistor Array</v>
+        <v>5V DC to DC Converter</v>
       </c>
       <c r="C10" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!C10),"",IF(ISBLANK(pyboardbreakout_data!D10),pyboardbreakout_data!C10,CONCATENATE(" :download:`",pyboardbreakout_data!C10,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D10,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`TBD62083AFNG&lt;../../manufacturing/datasheets/transistor_array.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`R-78E5.0-1.0&lt;../../manufacturing/datasheets/dc_converter.pdf&gt;`</v>
       </c>
       <c r="D10" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F10),"",CONCATENATE("`",pyboardbreakout_data!E10," &lt;",pyboardbreakout_data!F10,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/toshiba-semiconductor-and-storage/TBD62083AFNGEL/TBD62083AFNGELCT-ND/5514123&gt;`__</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=945-2201-ND&gt;`__</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="str">
         <f>pyboardbreakout_data!A11</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B11" t="str">
         <f>pyboardbreakout_data!B11</f>
-        <v>Diode</v>
+        <v>Transistor Array</v>
       </c>
       <c r="C11" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!C11),"",IF(ISBLANK(pyboardbreakout_data!D11),pyboardbreakout_data!C11,CONCATENATE(" :download:`",pyboardbreakout_data!C11,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D11,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`MBR120VLSFT3G&lt;../../manufacturing/datasheets/diode.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`TBD62083AFNG&lt;../../manufacturing/datasheets/transistor_array.pdf&gt;`</v>
       </c>
       <c r="D11" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F11),"",CONCATENATE("`",pyboardbreakout_data!E11," &lt;",pyboardbreakout_data!F11,"&gt;`__"))</f>
-        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/on-semiconductor/MBR120VLSFT3G/MBR120VLSFT3GOSCT-ND/3487322&gt;`__</v>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/toshiba-semiconductor-and-storage/TBD62083AFNGEL/TBD62083AFNGELCT-ND/5514123&gt;`__</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="str">
         <f>pyboardbreakout_data!A12</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="str">
         <f>pyboardbreakout_data!B12</f>
-        <v>10µF 25V Capacitor (1206)</v>
+        <v>Diode</v>
       </c>
       <c r="C12" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!C12),"",IF(ISBLANK(pyboardbreakout_data!D12),pyboardbreakout_data!C12,CONCATENATE(" :download:`",pyboardbreakout_data!C12,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D12,"&gt;`")))</f>
-        <v/>
+        <v xml:space="preserve"> :download:`MBR120VLSFT3G&lt;../../manufacturing/datasheets/diode.pdf&gt;`</v>
       </c>
       <c r="D12" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F12),"",CONCATENATE("`",pyboardbreakout_data!E12," &lt;",pyboardbreakout_data!F12,"&gt;`__"))</f>
+        <v>`Digi-Key &lt;https://www.digikey.com/product-detail/en/on-semiconductor/MBR120VLSFT3G/MBR120VLSFT3GOSCT-ND/3487322&gt;`__</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="str">
+        <f>pyboardbreakout_data!A13</f>
+        <v>2</v>
+      </c>
+      <c r="B13" t="str">
+        <f>pyboardbreakout_data!B13</f>
+        <v>10µF 25V Capacitor (1206)</v>
+      </c>
+      <c r="C13" t="str">
+        <f>IF(ISBLANK(pyboardbreakout_data!C13),"",IF(ISBLANK(pyboardbreakout_data!D13),pyboardbreakout_data!C13,CONCATENATE(" :download:`",pyboardbreakout_data!C13,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D13,"&gt;`")))</f>
+        <v/>
+      </c>
+      <c r="D13" t="str">
+        <f>IF(ISBLANK(pyboardbreakout_data!F13),"",CONCATENATE("`",pyboardbreakout_data!E13," &lt;",pyboardbreakout_data!F13,"&gt;`__"))</f>
         <v>`Digi-Key &lt;https://www.digikey.com/products/en?keywords=1276-1804-1-ND&gt;`__</v>
       </c>
     </row>
@@ -826,10 +856,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F120"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1008,87 +1038,102 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>1</v>
+      <c r="A9" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
+      <c r="A10" s="2">
+        <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C13" s="3"/>
-      <c r="F13"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="E18" s="4"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C14" s="3"/>
+      <c r="F14"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="5"/>
@@ -1096,6 +1141,8 @@
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
@@ -1110,8 +1157,8 @@
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E24" s="4"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C28" s="6"/>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E25" s="4"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C29" s="6"/>
@@ -1146,21 +1193,24 @@
     <row r="39" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C39" s="6"/>
     </row>
-    <row r="120" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F120" s="3"/>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C40" s="6"/>
+    </row>
+    <row r="121" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F121" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F10" r:id="rId1" xr:uid="{4D814F7E-E809-044B-A9CF-7ABAEE328861}"/>
+    <hyperlink ref="F11" r:id="rId1" xr:uid="{4D814F7E-E809-044B-A9CF-7ABAEE328861}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{05B760F1-2263-9849-9E96-16FABD4435DD}"/>
     <hyperlink ref="F4" r:id="rId3" display="https://www.digikey.com/products/en?keywords=B3F-4000" xr:uid="{297095E6-C369-9C43-87E4-9EE7FC3E90F5}"/>
     <hyperlink ref="F7" r:id="rId4" xr:uid="{A882F800-A73F-C940-828A-850803EE1E9B}"/>
-    <hyperlink ref="F11" r:id="rId5" xr:uid="{A4565103-D08B-9C42-B67C-AD72348CE1F4}"/>
-    <hyperlink ref="F9" r:id="rId6" display="https://www.digikey.com/product-detail/en/on-semiconductor/MC7805BDTRKG/MC7805BDTRKGOSCT-ND/1139742" xr:uid="{84379817-83EA-074E-96CF-155977A8D9F8}"/>
+    <hyperlink ref="F12" r:id="rId5" xr:uid="{A4565103-D08B-9C42-B67C-AD72348CE1F4}"/>
+    <hyperlink ref="F10" r:id="rId6" display="https://www.digikey.com/product-detail/en/on-semiconductor/MC7805BDTRKG/MC7805BDTRKGOSCT-ND/1139742" xr:uid="{84379817-83EA-074E-96CF-155977A8D9F8}"/>
     <hyperlink ref="F8" r:id="rId7" xr:uid="{38251BF6-DAAA-094A-96E3-B456AE1F7870}"/>
     <hyperlink ref="F5" r:id="rId8" xr:uid="{545989D7-5B32-5E4D-B4BD-757D46D9341E}"/>
     <hyperlink ref="F2" r:id="rId9" display="https://oshpark.com/shared_projects/x12GQ4xq" xr:uid="{F603E055-EBEC-EB49-8C97-D0FCC8E14D99}"/>
-    <hyperlink ref="F12" r:id="rId10" xr:uid="{079AE725-A048-B84F-ACEE-69047962AE7F}"/>
+    <hyperlink ref="F13" r:id="rId10" xr:uid="{079AE725-A048-B84F-ACEE-69047962AE7F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
PCB rev 1.4 removed mounting pads from D40 Hirose connector since that version of connector is discontinued. shifted pyboard connectors down and to the left so now an SD card can be inserted without interfering with microusb connector micro usb tx/rx were incorrectly wired. swapped buttons so user button is now closer to board edge (less likely to accidentally press reset on way to pressing user button).
</commit_message>
<xml_diff>
--- a/manufacturing/BOM.xlsx
+++ b/manufacturing/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/pyControl/DSeries_breakout/manufacturing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lustiga/Dropbox (HHMI)/Code/karpova_lab/pyControl/Hardware Modules/DSeries_breakout/manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CF704A-ED42-1941-8216-20B734A6E0F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A06DDA-9699-E348-804D-64D9439C5F2E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="460" windowWidth="24000" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t>Qty</t>
   </si>
@@ -172,12 +172,6 @@
     <t>breakout.pdf</t>
   </si>
   <si>
-    <t>https://oshpark.com/shared_projects/J8Bqlr2I</t>
-  </si>
-  <si>
-    <t>pyControl D-Series Breakout 1.2</t>
-  </si>
-  <si>
     <t>Printed Circuit Board</t>
   </si>
   <si>
@@ -212,6 +206,12 @@
   </si>
   <si>
     <t>Micro USB horizontal socket</t>
+  </si>
+  <si>
+    <t>pyControl D-Series Breakout 1.4</t>
+  </si>
+  <si>
+    <t>https://oshpark.com/shared_projects/qB3NMaHN</t>
   </si>
 </sst>
 </file>
@@ -600,7 +600,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,11 +640,11 @@
       </c>
       <c r="C2" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!C2),"",IF(ISBLANK(pyboardbreakout_data!D2),pyboardbreakout_data!C2,CONCATENATE(" :download:`",pyboardbreakout_data!C2,"&lt;../../manufacturing/datasheets/",pyboardbreakout_data!D2,"&gt;`")))</f>
-        <v xml:space="preserve"> :download:`pyControl D-Series Breakout 1.2&lt;../../manufacturing/datasheets/breakout.pdf&gt;`</v>
+        <v xml:space="preserve"> :download:`pyControl D-Series Breakout 1.4&lt;../../manufacturing/datasheets/breakout.pdf&gt;`</v>
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(pyboardbreakout_data!F2),"",CONCATENATE("`",pyboardbreakout_data!E2," &lt;",pyboardbreakout_data!F2,"&gt;`__"))</f>
-        <v>`OSH Park &lt;https://oshpark.com/shared_projects/J8Bqlr2I&gt;`__</v>
+        <v>`OSH Park &lt;https://oshpark.com/shared_projects/qB3NMaHN&gt;`__</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -720,9 +720,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <f>pyboardbreakout_data!A7</f>
-        <v>2</v>
+      <c r="A7" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B7" t="str">
         <f>pyboardbreakout_data!B7</f>
@@ -859,7 +858,7 @@
   <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -902,10 +901,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>44</v>
@@ -914,7 +913,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -945,7 +944,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>35</v>
@@ -954,7 +953,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -982,19 +981,19 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1042,19 +1041,19 @@
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1074,7 +1073,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>